<commit_message>
Added a utils folder with a csvToNdjson.js file for converting .csv data to .ndjson data so I can import it into sanity.
</commit_message>
<xml_diff>
--- a/data/events.xlsx
+++ b/data/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\code\rmlbb2-cms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{66A0C35F-2E8D-42F6-A152-DC79A5A713F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A84A2-CC06-4A20-8107-33666AB7A112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="151">
   <si>
     <t>Second Trading Period Begins</t>
   </si>
@@ -467,12 +467,18 @@
   </si>
   <si>
     <t>Everyone must download new lzp with roster changes.</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1312,23 +1318,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D213"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C138" sqref="C138"/>
+      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>132</v>
       </c>
@@ -1341,8 +1347,11 @@
       <c r="D1" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1352,8 +1361,11 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1363,8 +1375,11 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1374,8 +1389,11 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1385,8 +1403,11 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1396,8 +1417,11 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1407,8 +1431,11 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1418,8 +1445,11 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1429,8 +1459,11 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1440,8 +1473,11 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1451,8 +1487,11 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1462,8 +1501,11 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1473,8 +1515,11 @@
       <c r="C13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1487,8 +1532,11 @@
       <c r="D14" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1498,8 +1546,11 @@
       <c r="C15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1509,8 +1560,11 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1520,8 +1574,11 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1531,8 +1588,11 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1542,8 +1602,11 @@
       <c r="C19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1553,8 +1616,11 @@
       <c r="C20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1564,8 +1630,11 @@
       <c r="C21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1575,8 +1644,11 @@
       <c r="C22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1586,8 +1658,11 @@
       <c r="C23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1597,8 +1672,11 @@
       <c r="C24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1608,8 +1686,11 @@
       <c r="C25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1619,8 +1700,11 @@
       <c r="C26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1630,8 +1714,11 @@
       <c r="C27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1641,8 +1728,11 @@
       <c r="C28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1652,8 +1742,11 @@
       <c r="C29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1663,8 +1756,11 @@
       <c r="C30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1674,8 +1770,11 @@
       <c r="C31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1685,8 +1784,11 @@
       <c r="C32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1696,8 +1798,11 @@
       <c r="C33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1707,8 +1812,11 @@
       <c r="C34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1718,8 +1826,11 @@
       <c r="C35" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1729,8 +1840,11 @@
       <c r="C36" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1740,8 +1854,11 @@
       <c r="C37" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1751,8 +1868,11 @@
       <c r="C38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1762,8 +1882,11 @@
       <c r="C39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1773,8 +1896,11 @@
       <c r="C40" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1784,8 +1910,11 @@
       <c r="C41" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1795,8 +1924,11 @@
       <c r="C42" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1806,8 +1938,11 @@
       <c r="C43" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1817,8 +1952,11 @@
       <c r="C44" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1831,8 +1969,11 @@
       <c r="D45" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1842,8 +1983,11 @@
       <c r="C46" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1853,8 +1997,11 @@
       <c r="C47" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1867,8 +2014,11 @@
       <c r="D48" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1881,8 +2031,11 @@
       <c r="D49" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1892,8 +2045,11 @@
       <c r="C50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1903,8 +2059,11 @@
       <c r="C51" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1914,8 +2073,11 @@
       <c r="C52" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1925,8 +2087,11 @@
       <c r="C53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1936,8 +2101,11 @@
       <c r="C54" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1947,8 +2115,11 @@
       <c r="C55" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1961,8 +2132,11 @@
       <c r="D56" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1972,8 +2146,11 @@
       <c r="C57" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1983,8 +2160,11 @@
       <c r="C58" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1994,8 +2174,11 @@
       <c r="C59" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2005,8 +2188,11 @@
       <c r="C60" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2016,8 +2202,11 @@
       <c r="C61" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2027,8 +2216,11 @@
       <c r="C62" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2038,8 +2230,11 @@
       <c r="C63" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2049,8 +2244,11 @@
       <c r="C64" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2060,8 +2258,11 @@
       <c r="C65" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2071,8 +2272,11 @@
       <c r="C66" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2082,8 +2286,11 @@
       <c r="C67" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2093,8 +2300,11 @@
       <c r="C68" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2104,8 +2314,11 @@
       <c r="C69" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2115,8 +2328,11 @@
       <c r="C70" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2126,8 +2342,11 @@
       <c r="C71" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2137,8 +2356,11 @@
       <c r="C72" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>73</v>
       </c>
@@ -2148,8 +2370,11 @@
       <c r="C73" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>74</v>
       </c>
@@ -2159,8 +2384,11 @@
       <c r="C74" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>75</v>
       </c>
@@ -2170,8 +2398,11 @@
       <c r="C75" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>76</v>
       </c>
@@ -2181,8 +2412,11 @@
       <c r="C76" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>77</v>
       </c>
@@ -2192,8 +2426,11 @@
       <c r="C77" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>78</v>
       </c>
@@ -2203,8 +2440,11 @@
       <c r="C78" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>79</v>
       </c>
@@ -2217,8 +2457,11 @@
       <c r="D79" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>80</v>
       </c>
@@ -2228,8 +2471,11 @@
       <c r="C80" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>81</v>
       </c>
@@ -2239,8 +2485,11 @@
       <c r="C81" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>82</v>
       </c>
@@ -2250,8 +2499,11 @@
       <c r="C82" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>83</v>
       </c>
@@ -2261,8 +2513,11 @@
       <c r="C83" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>84</v>
       </c>
@@ -2272,8 +2527,11 @@
       <c r="C84" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>85</v>
       </c>
@@ -2283,8 +2541,11 @@
       <c r="C85" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>86</v>
       </c>
@@ -2297,8 +2558,11 @@
       <c r="D86" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>87</v>
       </c>
@@ -2308,8 +2572,11 @@
       <c r="C87" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>88</v>
       </c>
@@ -2319,8 +2586,11 @@
       <c r="C88" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>89</v>
       </c>
@@ -2330,8 +2600,11 @@
       <c r="C89" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>90</v>
       </c>
@@ -2341,8 +2614,11 @@
       <c r="C90" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>91</v>
       </c>
@@ -2352,8 +2628,11 @@
       <c r="C91" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>92</v>
       </c>
@@ -2363,8 +2642,11 @@
       <c r="C92" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>93</v>
       </c>
@@ -2374,8 +2656,11 @@
       <c r="C93" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>94</v>
       </c>
@@ -2385,8 +2670,11 @@
       <c r="C94" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>95</v>
       </c>
@@ -2396,8 +2684,11 @@
       <c r="C95" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>96</v>
       </c>
@@ -2407,8 +2698,11 @@
       <c r="C96" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>97</v>
       </c>
@@ -2418,8 +2712,11 @@
       <c r="C97" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>98</v>
       </c>
@@ -2429,8 +2726,11 @@
       <c r="C98" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>99</v>
       </c>
@@ -2440,8 +2740,11 @@
       <c r="C99" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>100</v>
       </c>
@@ -2451,8 +2754,11 @@
       <c r="C100" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>101</v>
       </c>
@@ -2462,8 +2768,11 @@
       <c r="C101" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>102</v>
       </c>
@@ -2473,8 +2782,11 @@
       <c r="C102" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>103</v>
       </c>
@@ -2484,8 +2796,11 @@
       <c r="C103" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>104</v>
       </c>
@@ -2495,8 +2810,11 @@
       <c r="C104" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>105</v>
       </c>
@@ -2506,8 +2824,11 @@
       <c r="C105" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>106</v>
       </c>
@@ -2517,8 +2838,11 @@
       <c r="C106" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>107</v>
       </c>
@@ -2528,8 +2852,11 @@
       <c r="C107" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>108</v>
       </c>
@@ -2539,8 +2866,11 @@
       <c r="C108" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>109</v>
       </c>
@@ -2550,8 +2880,11 @@
       <c r="C109" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>110</v>
       </c>
@@ -2564,8 +2897,11 @@
       <c r="D110" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>111</v>
       </c>
@@ -2575,8 +2911,11 @@
       <c r="C111" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>112</v>
       </c>
@@ -2586,8 +2925,11 @@
       <c r="C112" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>113</v>
       </c>
@@ -2597,8 +2939,11 @@
       <c r="C113" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>114</v>
       </c>
@@ -2608,8 +2953,11 @@
       <c r="C114" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E114" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>115</v>
       </c>
@@ -2619,8 +2967,11 @@
       <c r="C115" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E115" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>116</v>
       </c>
@@ -2630,8 +2981,11 @@
       <c r="C116" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>117</v>
       </c>
@@ -2641,8 +2995,11 @@
       <c r="C117" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>118</v>
       </c>
@@ -2652,8 +3009,11 @@
       <c r="C118" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E118" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>119</v>
       </c>
@@ -2663,8 +3023,11 @@
       <c r="C119" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E119" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>120</v>
       </c>
@@ -2674,8 +3037,11 @@
       <c r="C120" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E120" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>121</v>
       </c>
@@ -2685,8 +3051,11 @@
       <c r="C121" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E121" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>122</v>
       </c>
@@ -2696,8 +3065,11 @@
       <c r="C122" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E122" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>123</v>
       </c>
@@ -2707,8 +3079,11 @@
       <c r="C123" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E123" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>124</v>
       </c>
@@ -2718,8 +3093,11 @@
       <c r="C124" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>125</v>
       </c>
@@ -2729,8 +3107,11 @@
       <c r="C125" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>126</v>
       </c>
@@ -2740,8 +3121,11 @@
       <c r="C126" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E126" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>127</v>
       </c>
@@ -2751,8 +3135,11 @@
       <c r="C127" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E127" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>128</v>
       </c>
@@ -2762,8 +3149,11 @@
       <c r="C128" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>129</v>
       </c>
@@ -2773,8 +3163,11 @@
       <c r="C129" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>130</v>
       </c>
@@ -2784,8 +3177,11 @@
       <c r="C130" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>131</v>
       </c>
@@ -2795,8 +3191,11 @@
       <c r="C131" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>132</v>
       </c>
@@ -2806,8 +3205,11 @@
       <c r="C132" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>133</v>
       </c>
@@ -2817,8 +3219,11 @@
       <c r="C133" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>134</v>
       </c>
@@ -2828,8 +3233,11 @@
       <c r="C134" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>135</v>
       </c>
@@ -2839,8 +3247,11 @@
       <c r="C135" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>136</v>
       </c>
@@ -2850,8 +3261,11 @@
       <c r="C136" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>137</v>
       </c>
@@ -2864,8 +3278,11 @@
       <c r="D137" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>138</v>
       </c>
@@ -2875,8 +3292,11 @@
       <c r="C138" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>139</v>
       </c>
@@ -2886,8 +3306,11 @@
       <c r="C139" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>140</v>
       </c>
@@ -2897,8 +3320,11 @@
       <c r="C140" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>141</v>
       </c>
@@ -2908,8 +3334,11 @@
       <c r="C141" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>142</v>
       </c>
@@ -2919,8 +3348,11 @@
       <c r="C142" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>143</v>
       </c>
@@ -2930,8 +3362,11 @@
       <c r="C143" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>144</v>
       </c>
@@ -2941,8 +3376,11 @@
       <c r="C144" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>145</v>
       </c>
@@ -2952,8 +3390,11 @@
       <c r="C145" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>146</v>
       </c>
@@ -2963,8 +3404,11 @@
       <c r="C146" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>147</v>
       </c>
@@ -2974,8 +3418,11 @@
       <c r="C147" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>148</v>
       </c>
@@ -2985,8 +3432,11 @@
       <c r="C148" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>149</v>
       </c>
@@ -2996,8 +3446,11 @@
       <c r="C149" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>150</v>
       </c>
@@ -3007,8 +3460,11 @@
       <c r="C150" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>151</v>
       </c>
@@ -3018,8 +3474,11 @@
       <c r="C151" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>152</v>
       </c>
@@ -3029,8 +3488,11 @@
       <c r="C152" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>153</v>
       </c>
@@ -3040,8 +3502,11 @@
       <c r="C153" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>154</v>
       </c>
@@ -3051,8 +3516,11 @@
       <c r="C154" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>155</v>
       </c>
@@ -3062,8 +3530,11 @@
       <c r="C155" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>156</v>
       </c>
@@ -3073,8 +3544,11 @@
       <c r="C156" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>157</v>
       </c>
@@ -3084,8 +3558,11 @@
       <c r="C157" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>158</v>
       </c>
@@ -3095,8 +3572,11 @@
       <c r="C158" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>159</v>
       </c>
@@ -3106,8 +3586,11 @@
       <c r="C159" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>160</v>
       </c>
@@ -3120,8 +3603,11 @@
       <c r="D160" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E160" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>161</v>
       </c>
@@ -3131,8 +3617,11 @@
       <c r="C161" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E161" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>162</v>
       </c>
@@ -3142,8 +3631,11 @@
       <c r="C162" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E162" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>163</v>
       </c>
@@ -3153,8 +3645,11 @@
       <c r="C163" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E163" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>164</v>
       </c>
@@ -3164,8 +3659,11 @@
       <c r="C164" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E164" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>165</v>
       </c>
@@ -3175,8 +3673,11 @@
       <c r="C165" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E165" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>166</v>
       </c>
@@ -3186,8 +3687,11 @@
       <c r="C166" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E166" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>167</v>
       </c>
@@ -3197,8 +3701,11 @@
       <c r="C167" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E167" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>168</v>
       </c>
@@ -3208,8 +3715,11 @@
       <c r="C168" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E168" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>169</v>
       </c>
@@ -3219,8 +3729,11 @@
       <c r="C169" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E169" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>170</v>
       </c>
@@ -3230,8 +3743,11 @@
       <c r="C170" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E170" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>171</v>
       </c>
@@ -3241,8 +3757,11 @@
       <c r="C171" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E171" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>172</v>
       </c>
@@ -3252,8 +3771,11 @@
       <c r="C172" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E172" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>173</v>
       </c>
@@ -3263,8 +3785,11 @@
       <c r="C173" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E173" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>174</v>
       </c>
@@ -3274,8 +3799,11 @@
       <c r="C174" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E174" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>175</v>
       </c>
@@ -3285,8 +3813,11 @@
       <c r="C175" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E175" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>176</v>
       </c>
@@ -3296,8 +3827,11 @@
       <c r="C176" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>177</v>
       </c>
@@ -3307,8 +3841,11 @@
       <c r="C177" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>178</v>
       </c>
@@ -3318,8 +3855,11 @@
       <c r="C178" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>179</v>
       </c>
@@ -3329,8 +3869,11 @@
       <c r="C179" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>180</v>
       </c>
@@ -3340,8 +3883,11 @@
       <c r="C180" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>181</v>
       </c>
@@ -3351,8 +3897,11 @@
       <c r="C181" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>182</v>
       </c>
@@ -3362,8 +3911,11 @@
       <c r="C182" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>183</v>
       </c>
@@ -3373,8 +3925,11 @@
       <c r="C183" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>184</v>
       </c>
@@ -3384,8 +3939,11 @@
       <c r="C184" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>185</v>
       </c>
@@ -3395,8 +3953,11 @@
       <c r="C185" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>186</v>
       </c>
@@ -3406,8 +3967,11 @@
       <c r="C186" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>187</v>
       </c>
@@ -3417,8 +3981,11 @@
       <c r="C187" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>188</v>
       </c>
@@ -3428,8 +3995,11 @@
       <c r="C188" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>189</v>
       </c>
@@ -3439,8 +4009,11 @@
       <c r="C189" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>190</v>
       </c>
@@ -3450,8 +4023,11 @@
       <c r="C190" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>191</v>
       </c>
@@ -3464,8 +4040,11 @@
       <c r="D191" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>192</v>
       </c>
@@ -3475,8 +4054,11 @@
       <c r="C192" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E192" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>193</v>
       </c>
@@ -3486,8 +4068,11 @@
       <c r="C193" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E193" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>194</v>
       </c>
@@ -3497,8 +4082,11 @@
       <c r="C194" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E194" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>195</v>
       </c>
@@ -3508,8 +4096,11 @@
       <c r="C195" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E195" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>196</v>
       </c>
@@ -3519,8 +4110,11 @@
       <c r="C196" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E196" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>197</v>
       </c>
@@ -3530,8 +4124,11 @@
       <c r="C197" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E197" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>198</v>
       </c>
@@ -3541,8 +4138,11 @@
       <c r="C198" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E198" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>199</v>
       </c>
@@ -3552,8 +4152,11 @@
       <c r="C199" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E199" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>200</v>
       </c>
@@ -3563,8 +4166,11 @@
       <c r="C200" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E200" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>201</v>
       </c>
@@ -3574,8 +4180,11 @@
       <c r="C201" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E201" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>202</v>
       </c>
@@ -3585,8 +4194,11 @@
       <c r="C202" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E202" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>203</v>
       </c>
@@ -3596,8 +4208,11 @@
       <c r="C203" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E203" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>204</v>
       </c>
@@ -3607,8 +4222,11 @@
       <c r="C204" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E204" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>205</v>
       </c>
@@ -3618,8 +4236,11 @@
       <c r="C205" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E205" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>206</v>
       </c>
@@ -3629,8 +4250,11 @@
       <c r="C206" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E206" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>207</v>
       </c>
@@ -3640,8 +4264,11 @@
       <c r="C207" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E207" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>208</v>
       </c>
@@ -3651,8 +4278,11 @@
       <c r="C208" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E208" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>209</v>
       </c>
@@ -3662,8 +4292,11 @@
       <c r="C209" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E209" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>210</v>
       </c>
@@ -3673,8 +4306,11 @@
       <c r="C210" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E210" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>211</v>
       </c>
@@ -3684,8 +4320,11 @@
       <c r="C211" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E211" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>212</v>
       </c>
@@ -3695,8 +4334,11 @@
       <c r="C212" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E212" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>213</v>
       </c>
@@ -3705,6 +4347,9 @@
       </c>
       <c r="C213" t="s">
         <v>129</v>
+      </c>
+      <c r="E213" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>